<commit_message>
Update DateBase/orders/International Ever Green_2025-11-24.xlsx
</commit_message>
<xml_diff>
--- a/DateBase/orders/International Ever Green_2025-11-24.xlsx
+++ b/DateBase/orders/International Ever Green_2025-11-24.xlsx
@@ -777,6 +777,9 @@
       <c r="C41" t="str">
         <v>431_小米果_undefined_undefined_1bunch</v>
       </c>
+      <c r="F41" t="str">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <ignoredErrors>
@@ -838,7 +841,7 @@
         <v>0.00</v>
       </c>
       <c r="G2" t="str">
-        <v>0551555525106525665555253215158225555105555512551560</v>
+        <v>0551555525106525665555253215158225555105555512551565</v>
       </c>
     </row>
   </sheetData>

</xml_diff>